<commit_message>
made many changes across the project
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -114,10 +114,7 @@
     <t>22, LimeSquare, City Road</t>
   </si>
   <si>
-    <t>testuser_2</t>
-  </si>
-  <si>
-    <t>Test@223</t>
+    <t>Fail</t>
   </si>
   <si>
     <t>Pass</t>
@@ -167,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -201,46 +198,30 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -254,10 +235,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -415,7 +396,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -424,13 +405,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -440,7 +421,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -449,7 +430,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -458,7 +439,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -468,12 +449,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -504,7 +485,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -523,7 +504,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -535,31 +516,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="1" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -575,25 +553,25 @@
       <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="M1" s="5" t="s">
@@ -640,11 +618,11 @@
       <c r="L2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -652,10 +630,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -684,51 +662,53 @@
       <c r="L3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="N3" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E3" type="list">
       <formula1>"Accessories, iMacs, iPads, iPhones"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F2:F3" type="list">
       <formula1>"Product 1, Product 2, Product 3, Product 4"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId6"/>
-    <hyperlink ref="M2" r:id="rId7"/>
-    <hyperlink ref="C3" r:id="rId8"/>
-    <hyperlink ref="M3" r:id="rId9"/>
+    <hyperlink r:id="rId22" ref="C2"/>
+    <hyperlink r:id="rId23" ref="M2"/>
+    <hyperlink r:id="rId24" ref="C3"/>
+    <hyperlink r:id="rId25" ref="M3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>